<commit_message>
Add test for unsupported icon sets
</commit_message>
<xml_diff>
--- a/tests/data/Reader/XLSX/conditionalFormattingIconSet.xlsx
+++ b/tests/data/Reader/XLSX/conditionalFormattingIconSet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>type: 3Arrows
 reverse: false
@@ -89,6 +89,23 @@
     <t>type: 3Flags
 reverse: false
 showValue: true</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>type: 3Stars</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>type: 3Triangles</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>type: 5Boxes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>type: NoIcons
+custom: true</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -446,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -454,13 +471,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="131.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="131.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,8 +529,20 @@
       <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -565,8 +594,20 @@
       <c r="Q2">
         <v>1</v>
       </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -618,8 +659,20 @@
       <c r="Q3">
         <v>2</v>
       </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>8</v>
       </c>
@@ -671,8 +724,20 @@
       <c r="Q4">
         <v>8</v>
       </c>
+      <c r="R4">
+        <v>8</v>
+      </c>
+      <c r="S4">
+        <v>8</v>
+      </c>
+      <c r="T4">
+        <v>8</v>
+      </c>
+      <c r="U4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -724,8 +789,20 @@
       <c r="Q5">
         <v>4</v>
       </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -777,8 +854,20 @@
       <c r="Q6">
         <v>5</v>
       </c>
+      <c r="R6">
+        <v>5</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+      <c r="T6">
+        <v>5</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -830,8 +919,20 @@
       <c r="Q7">
         <v>6</v>
       </c>
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <v>6</v>
+      </c>
+      <c r="T7">
+        <v>6</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -883,8 +984,20 @@
       <c r="Q8">
         <v>7</v>
       </c>
+      <c r="R8">
+        <v>7</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8">
+        <v>7</v>
+      </c>
+      <c r="U8">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>3</v>
       </c>
@@ -936,8 +1049,20 @@
       <c r="Q9">
         <v>3</v>
       </c>
+      <c r="R9">
+        <v>3</v>
+      </c>
+      <c r="S9">
+        <v>3</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -989,8 +1114,20 @@
       <c r="Q10">
         <v>9</v>
       </c>
+      <c r="R10">
+        <v>9</v>
+      </c>
+      <c r="S10">
+        <v>9</v>
+      </c>
+      <c r="T10">
+        <v>9</v>
+      </c>
+      <c r="U10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1040,13 +1177,25 @@
         <v>10</v>
       </c>
       <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
+      </c>
+      <c r="S11">
+        <v>10</v>
+      </c>
+      <c r="T11">
+        <v>10</v>
+      </c>
+      <c r="U11">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="A2:A11">
-    <cfRule type="iconSet" priority="21">
+    <cfRule type="iconSet" priority="25">
       <iconSet iconSet="3Arrows" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33" gte="0"/>
@@ -1055,7 +1204,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="iconSet" priority="22">
+    <cfRule type="iconSet" priority="26">
       <iconSet iconSet="3ArrowsGray" showValue="0" reverse="1">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="3" gte="0"/>
@@ -1064,7 +1213,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="iconSet" priority="23">
+    <cfRule type="iconSet" priority="27">
       <iconSet iconSet="3Flags">
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="10/3" gte="0"/>
@@ -1073,7 +1222,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="iconSet" priority="24">
+    <cfRule type="iconSet" priority="28">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="33" gte="0"/>
@@ -1082,7 +1231,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="iconSet" priority="25">
+    <cfRule type="iconSet" priority="29">
       <iconSet iconSet="3TrafficLights2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1091,7 +1240,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="iconSet" priority="26">
+    <cfRule type="iconSet" priority="30">
       <iconSet iconSet="3Signs">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1100,7 +1249,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="iconSet" priority="27">
+    <cfRule type="iconSet" priority="31">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1109,7 +1258,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="iconSet" priority="28">
+    <cfRule type="iconSet" priority="32">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1118,7 +1267,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="iconSet" priority="29">
+    <cfRule type="iconSet" priority="33">
       <iconSet iconSet="4Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -1128,7 +1277,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="iconSet" priority="30">
+    <cfRule type="iconSet" priority="34">
       <iconSet iconSet="4ArrowsGray">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -1138,7 +1287,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="iconSet" priority="31">
+    <cfRule type="iconSet" priority="35">
       <iconSet iconSet="4RedToBlack">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -1148,7 +1297,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L11">
-    <cfRule type="iconSet" priority="32">
+    <cfRule type="iconSet" priority="36">
       <iconSet iconSet="4Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -1158,7 +1307,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M11">
-    <cfRule type="iconSet" priority="33">
+    <cfRule type="iconSet" priority="37">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -1168,7 +1317,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N11">
-    <cfRule type="iconSet" priority="34">
+    <cfRule type="iconSet" priority="38">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -1179,7 +1328,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O11">
-    <cfRule type="iconSet" priority="35">
+    <cfRule type="iconSet" priority="39">
       <iconSet iconSet="5ArrowsGray">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -1190,7 +1339,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P11">
-    <cfRule type="iconSet" priority="36">
+    <cfRule type="iconSet" priority="40">
       <iconSet iconSet="5Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -1201,7 +1350,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q11">
-    <cfRule type="iconSet" priority="37">
+    <cfRule type="iconSet" priority="41">
       <iconSet iconSet="5Quarters">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -1213,5 +1362,84 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{A7B15CCB-3CA5-4F93-9228-B37B90BBED97}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>R2:R11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{3C6CBD8E-7ED5-4213-A63B-8BAFEDCE63C6}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>S2:S11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{3675D329-1519-490F-A5C2-711B90CA345D}">
+            <x14:iconSet iconSet="5Boxes">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>20</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>40</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>80</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>T2:T11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{284D1E99-5529-431E-8D9F-13027492D7EE}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>U2:U11</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>